<commit_message>
Finally added the page to show the actual monthly salaries, reorganized some code and reorganized the navbar
</commit_message>
<xml_diff>
--- a/data comparisons.xlsx
+++ b/data comparisons.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="26">
   <si>
     <t>Person Name</t>
   </si>
@@ -83,12 +83,6 @@
     <t>compare results</t>
   </si>
   <si>
-    <t>so only last line in a group contains accurate data</t>
-  </si>
-  <si>
-    <t>orange grouped lines belong to the same day</t>
-  </si>
-  <si>
     <t>Janet total</t>
   </si>
   <si>
@@ -108,6 +102,9 @@
   </si>
   <si>
     <t>salaries</t>
+  </si>
+  <si>
+    <t>Belong to same day</t>
   </si>
 </sst>
 </file>
@@ -237,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -281,11 +278,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -293,20 +291,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -636,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -703,13 +687,13 @@
         <v>17</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
@@ -780,7 +764,7 @@
         <v>ok</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="R2" s="11">
         <f>SUM(M2:M24)-M5-M17</f>
@@ -792,7 +776,7 @@
       </c>
       <c r="T2" s="10"/>
       <c r="U2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="V2">
         <v>3.75</v>
@@ -865,7 +849,7 @@
         <v>ok</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R3" s="11">
         <f>SUM(M25:M49)-M32-M43</f>
@@ -928,7 +912,7 @@
         <v>ok</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R4" s="11">
         <f>SUM(M50:M68)-M57-M58</f>
@@ -1082,7 +1066,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="14">
-        <f>H7*$V$2+I7*$W$2+J7*$X$2+K7*$Y$2+L7*$Z$2</f>
+        <f t="shared" ref="M7:M17" si="3">H7*$V$2+I7*$W$2+J7*$X$2+K7*$Y$2+L7*$Z$2</f>
         <v>30</v>
       </c>
       <c r="N7" s="15">
@@ -1133,7 +1117,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="14">
-        <f>H8*$V$2+I8*$W$2+J8*$X$2+K8*$Y$2+L8*$Z$2</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="N8" s="15">
@@ -1184,7 +1168,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="14">
-        <f>H9*$V$2+I9*$W$2+J9*$X$2+K9*$Y$2+L9*$Z$2</f>
+        <f t="shared" si="3"/>
         <v>32.34375</v>
       </c>
       <c r="N9" s="15">
@@ -1235,7 +1219,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="14">
-        <f>H10*$V$2+I10*$W$2+J10*$X$2+K10*$Y$2+L10*$Z$2</f>
+        <f t="shared" si="3"/>
         <v>46.275000000000006</v>
       </c>
       <c r="N10" s="15">
@@ -1245,6 +1229,10 @@
         <f t="shared" si="2"/>
         <v>ok</v>
       </c>
+      <c r="R10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
@@ -1286,7 +1274,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="14">
-        <f>H11*$V$2+I11*$W$2+J11*$X$2+K11*$Y$2+L11*$Z$2</f>
+        <f t="shared" si="3"/>
         <v>18.75</v>
       </c>
       <c r="N11" s="15">
@@ -1337,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="14">
-        <f>H12*$V$2+I12*$W$2+J12*$X$2+K12*$Y$2+L12*$Z$2</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="N12" s="15">
@@ -1388,7 +1376,7 @@
         <v>2</v>
       </c>
       <c r="M13" s="14">
-        <f>H13*$V$2+I13*$W$2+J13*$X$2+K13*$Y$2+L13*$Z$2</f>
+        <f t="shared" si="3"/>
         <v>65.625</v>
       </c>
       <c r="N13" s="15">
@@ -1398,15 +1386,13 @@
         <f t="shared" si="2"/>
         <v>ok</v>
       </c>
-      <c r="R13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="37"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="37"/>
+      <c r="W13" s="37"/>
+      <c r="X13" s="37"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1448,7 +1434,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="14">
-        <f>H14*$V$2+I14*$W$2+J14*$X$2+K14*$Y$2+L14*$Z$2</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="N14" s="15">
@@ -1458,15 +1444,13 @@
         <f t="shared" si="2"/>
         <v>ok</v>
       </c>
-      <c r="R14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="37"/>
+      <c r="U14" s="37"/>
+      <c r="V14" s="37"/>
+      <c r="W14" s="37"/>
+      <c r="X14" s="37"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
@@ -1508,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="14">
-        <f>H15*$V$2+I15*$W$2+J15*$X$2+K15*$Y$2+L15*$Z$2</f>
+        <f t="shared" si="3"/>
         <v>26.25</v>
       </c>
       <c r="N15" s="15">
@@ -1559,7 +1543,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="14">
-        <f>H16*$V$2+I16*$W$2+J16*$X$2+K16*$Y$2+L16*$Z$2</f>
+        <f t="shared" si="3"/>
         <v>26.25</v>
       </c>
       <c r="N16" s="15">
@@ -1610,7 +1594,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="31">
-        <f>H17*$V$2+I17*$W$2+J17*$X$2+K17*$Y$2+L17*$Z$2</f>
+        <f t="shared" si="3"/>
         <v>19.600000000000001</v>
       </c>
       <c r="N17" s="32"/>
@@ -1710,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="12">
-        <f>H19*$V$2+I19*$W$2+J19*$X$2+K19*$Y$2+L19*$Z$2</f>
+        <f t="shared" ref="M19:M32" si="4">H19*$V$2+I19*$W$2+J19*$X$2+K19*$Y$2+L19*$Z$2</f>
         <v>30</v>
       </c>
       <c r="N19" s="13">
@@ -1761,7 +1745,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="12">
-        <f>H20*$V$2+I20*$W$2+J20*$X$2+K20*$Y$2+L20*$Z$2</f>
+        <f t="shared" si="4"/>
         <v>29.0625</v>
       </c>
       <c r="N20" s="13">
@@ -1812,7 +1796,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="12">
-        <f>H21*$V$2+I21*$W$2+J21*$X$2+K21*$Y$2+L21*$Z$2</f>
+        <f t="shared" si="4"/>
         <v>34.6875</v>
       </c>
       <c r="N21" s="13">
@@ -1863,7 +1847,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="12">
-        <f>H22*$V$2+I22*$W$2+J22*$X$2+K22*$Y$2+L22*$Z$2</f>
+        <f t="shared" si="4"/>
         <v>27.1875</v>
       </c>
       <c r="N22" s="13">
@@ -1914,7 +1898,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="12">
-        <f>H23*$V$2+I23*$W$2+J23*$X$2+K23*$Y$2+L23*$Z$2</f>
+        <f t="shared" si="4"/>
         <v>29.0625</v>
       </c>
       <c r="N23" s="13">
@@ -1965,7 +1949,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="12">
-        <f>H24*$V$2+I24*$W$2+J24*$X$2+K24*$Y$2+L24*$Z$2</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="N24" s="13">
@@ -2016,7 +2000,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="12">
-        <f>H25*$V$2+I25*$W$2+J25*$X$2+K25*$Y$2+L25*$Z$2</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="N25" s="13">
@@ -2067,7 +2051,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="12">
-        <f>H26*$V$2+I26*$W$2+J26*$X$2+K26*$Y$2+L26*$Z$2</f>
+        <f t="shared" si="4"/>
         <v>29.0625</v>
       </c>
       <c r="N26" s="13">
@@ -2118,7 +2102,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="12">
-        <f>H27*$V$2+I27*$W$2+J27*$X$2+K27*$Y$2+L27*$Z$2</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="N27" s="13">
@@ -2169,7 +2153,7 @@
         <v>0</v>
       </c>
       <c r="M28" s="12">
-        <f>H28*$V$2+I28*$W$2+J28*$X$2+K28*$Y$2+L28*$Z$2</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="N28" s="13">
@@ -2220,7 +2204,7 @@
         <v>0</v>
       </c>
       <c r="M29" s="12">
-        <f>H29*$V$2+I29*$W$2+J29*$X$2+K29*$Y$2+L29*$Z$2</f>
+        <f t="shared" si="4"/>
         <v>33.515625</v>
       </c>
       <c r="N29" s="13">
@@ -2271,7 +2255,7 @@
         <v>0</v>
       </c>
       <c r="M30" s="12">
-        <f>H30*$V$2+I30*$W$2+J30*$X$2+K30*$Y$2+L30*$Z$2</f>
+        <f t="shared" si="4"/>
         <v>33.515625</v>
       </c>
       <c r="N30" s="13">
@@ -2322,7 +2306,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="12">
-        <f>H31*$V$2+I31*$W$2+J31*$X$2+K31*$Y$2+L31*$Z$2</f>
+        <f t="shared" si="4"/>
         <v>7.5</v>
       </c>
       <c r="N31" s="13">
@@ -2373,12 +2357,12 @@
         <v>0</v>
       </c>
       <c r="M32" s="34">
-        <f>H32*$V$2+I32*$W$2+J32*$X$2+K32*$Y$2+L32*$Z$2</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="N32" s="35"/>
       <c r="O32" s="36" t="str">
-        <f>IF(M32=N32, "ok", "mismatch")</f>
+        <f t="shared" ref="O32:O48" si="5">IF(M32=N32, "ok", "mismatch")</f>
         <v>mismatch</v>
       </c>
     </row>
@@ -2429,7 +2413,7 @@
         <v>34.6875</v>
       </c>
       <c r="O33" s="21" t="str">
-        <f>IF(M33=N33, "ok", "mismatch")</f>
+        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
     </row>
@@ -2473,14 +2457,14 @@
         <v>0</v>
       </c>
       <c r="M34" s="12">
-        <f>H34*$V$2+I34*$W$2+J34*$X$2+K34*$Y$2+L34*$Z$2</f>
+        <f t="shared" ref="M34:M43" si="6">H34*$V$2+I34*$W$2+J34*$X$2+K34*$Y$2+L34*$Z$2</f>
         <v>32.34375</v>
       </c>
       <c r="N34" s="13">
         <v>32.34375</v>
       </c>
       <c r="O34" s="21" t="str">
-        <f>IF(M34=N34, "ok", "mismatch")</f>
+        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
     </row>
@@ -2524,14 +2508,14 @@
         <v>0</v>
       </c>
       <c r="M35" s="12">
-        <f>H35*$V$2+I35*$W$2+J35*$X$2+K35*$Y$2+L35*$Z$2</f>
+        <f t="shared" si="6"/>
         <v>32.34375</v>
       </c>
       <c r="N35" s="13">
         <v>32.34375</v>
       </c>
       <c r="O35" s="21" t="str">
-        <f>IF(M35=N35, "ok", "mismatch")</f>
+        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
     </row>
@@ -2575,14 +2559,14 @@
         <v>0</v>
       </c>
       <c r="M36" s="12">
-        <f>H36*$V$2+I36*$W$2+J36*$X$2+K36*$Y$2+L36*$Z$2</f>
+        <f t="shared" si="6"/>
         <v>51.006250000000001</v>
       </c>
       <c r="N36" s="13">
         <v>51.006250000000001</v>
       </c>
       <c r="O36" s="21" t="str">
-        <f>IF(M36=N36, "ok", "mismatch")</f>
+        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
     </row>
@@ -2626,14 +2610,14 @@
         <v>0</v>
       </c>
       <c r="M37" s="12">
-        <f>H37*$V$2+I37*$W$2+J37*$X$2+K37*$Y$2+L37*$Z$2</f>
+        <f t="shared" si="6"/>
         <v>28.125</v>
       </c>
       <c r="N37" s="13">
         <v>28.125</v>
       </c>
       <c r="O37" s="21" t="str">
-        <f>IF(M37=N37, "ok", "mismatch")</f>
+        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
     </row>
@@ -2677,14 +2661,14 @@
         <v>0</v>
       </c>
       <c r="M38" s="12">
-        <f>H38*$V$2+I38*$W$2+J38*$X$2+K38*$Y$2+L38*$Z$2</f>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="N38" s="13">
         <v>30</v>
       </c>
       <c r="O38" s="21" t="str">
-        <f>IF(M38=N38, "ok", "mismatch")</f>
+        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
     </row>
@@ -2728,14 +2712,14 @@
         <v>0</v>
       </c>
       <c r="M39" s="12">
-        <f>H39*$V$2+I39*$W$2+J39*$X$2+K39*$Y$2+L39*$Z$2</f>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="N39" s="13">
         <v>30</v>
       </c>
       <c r="O39" s="21" t="str">
-        <f>IF(M39=N39, "ok", "mismatch")</f>
+        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
     </row>
@@ -2779,14 +2763,14 @@
         <v>0</v>
       </c>
       <c r="M40" s="12">
-        <f>H40*$V$2+I40*$W$2+J40*$X$2+K40*$Y$2+L40*$Z$2</f>
+        <f t="shared" si="6"/>
         <v>7.5</v>
       </c>
       <c r="N40" s="13">
         <v>7.5</v>
       </c>
       <c r="O40" s="21" t="str">
-        <f>IF(M40=N40, "ok", "mismatch")</f>
+        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
     </row>
@@ -2830,14 +2814,14 @@
         <v>0</v>
       </c>
       <c r="M41" s="12">
-        <f>H41*$V$2+I41*$W$2+J41*$X$2+K41*$Y$2+L41*$Z$2</f>
+        <f t="shared" si="6"/>
         <v>7.5</v>
       </c>
       <c r="N41" s="13">
         <v>7.5</v>
       </c>
       <c r="O41" s="21" t="str">
-        <f>IF(M41=N41, "ok", "mismatch")</f>
+        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
     </row>
@@ -2881,14 +2865,14 @@
         <v>0</v>
       </c>
       <c r="M42" s="12">
-        <f>H42*$V$2+I42*$W$2+J42*$X$2+K42*$Y$2+L42*$Z$2</f>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="N42" s="13">
         <v>30</v>
       </c>
       <c r="O42" s="21" t="str">
-        <f>IF(M42=N42, "ok", "mismatch")</f>
+        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
     </row>
@@ -2932,12 +2916,12 @@
         <v>0</v>
       </c>
       <c r="M43" s="34">
-        <f>H43*$V$2+I43*$W$2+J43*$X$2+K43*$Y$2+L43*$Z$2</f>
+        <f t="shared" si="6"/>
         <v>1.875</v>
       </c>
       <c r="N43" s="35"/>
       <c r="O43" s="36" t="str">
-        <f>IF(M43=N43, "ok", "mismatch")</f>
+        <f t="shared" si="5"/>
         <v>mismatch</v>
       </c>
     </row>
@@ -2988,7 +2972,7 @@
         <v>2.8125</v>
       </c>
       <c r="O44" s="21" t="str">
-        <f>IF(M44=N44, "ok", "mismatch")</f>
+        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
     </row>
@@ -3032,14 +3016,14 @@
         <v>0</v>
       </c>
       <c r="M45" s="12">
-        <f>H45*$V$2+I45*$W$2+J45*$X$2+K45*$Y$2+L45*$Z$2</f>
+        <f t="shared" ref="M45:M58" si="7">H45*$V$2+I45*$W$2+J45*$X$2+K45*$Y$2+L45*$Z$2</f>
         <v>39.200000000000003</v>
       </c>
       <c r="N45" s="13">
         <v>39.200000000000003</v>
       </c>
       <c r="O45" s="21" t="str">
-        <f>IF(M45=N45, "ok", "mismatch")</f>
+        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
     </row>
@@ -3083,14 +3067,14 @@
         <v>0</v>
       </c>
       <c r="M46" s="12">
-        <f>H46*$V$2+I46*$W$2+J46*$X$2+K46*$Y$2+L46*$Z$2</f>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="N46" s="13">
         <v>30</v>
       </c>
       <c r="O46" s="21" t="str">
-        <f>IF(M46=N46, "ok", "mismatch")</f>
+        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
     </row>
@@ -3134,14 +3118,14 @@
         <v>0</v>
       </c>
       <c r="M47" s="12">
-        <f>H47*$V$2+I47*$W$2+J47*$X$2+K47*$Y$2+L47*$Z$2</f>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="N47" s="13">
         <v>30</v>
       </c>
       <c r="O47" s="21" t="str">
-        <f>IF(M47=N47, "ok", "mismatch")</f>
+        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
     </row>
@@ -3185,14 +3169,14 @@
         <v>0</v>
       </c>
       <c r="M48" s="12">
-        <f>H48*$V$2+I48*$W$2+J48*$X$2+K48*$Y$2+L48*$Z$2</f>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="N48" s="13">
         <v>30</v>
       </c>
       <c r="O48" s="21" t="str">
-        <f>IF(M48=N48, "ok", "mismatch")</f>
+        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
     </row>
@@ -3236,7 +3220,7 @@
         <v>0</v>
       </c>
       <c r="M49" s="12">
-        <f>H49*$V$2+I49*$W$2+J49*$X$2+K49*$Y$2+L49*$Z$2</f>
+        <f t="shared" si="7"/>
         <v>42.1875</v>
       </c>
       <c r="N49" s="13">
@@ -3287,7 +3271,7 @@
         <v>0</v>
       </c>
       <c r="M50" s="12">
-        <f>H50*$V$2+I50*$W$2+J50*$X$2+K50*$Y$2+L50*$Z$2</f>
+        <f t="shared" si="7"/>
         <v>4.9000000000000004</v>
       </c>
       <c r="N50" s="13">
@@ -3338,7 +3322,7 @@
         <v>0</v>
       </c>
       <c r="M51" s="12">
-        <f>H51*$V$2+I51*$W$2+J51*$X$2+K51*$Y$2+L51*$Z$2</f>
+        <f t="shared" si="7"/>
         <v>19.899999999999999</v>
       </c>
       <c r="N51" s="13">
@@ -3389,7 +3373,7 @@
         <v>0</v>
       </c>
       <c r="M52" s="12">
-        <f>H52*$V$2+I52*$W$2+J52*$X$2+K52*$Y$2+L52*$Z$2</f>
+        <f t="shared" si="7"/>
         <v>19.899999999999999</v>
       </c>
       <c r="N52" s="13">
@@ -3440,7 +3424,7 @@
         <v>0</v>
       </c>
       <c r="M53" s="12">
-        <f>H53*$V$2+I53*$W$2+J53*$X$2+K53*$Y$2+L53*$Z$2</f>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="N53" s="13">
@@ -3491,7 +3475,7 @@
         <v>0</v>
       </c>
       <c r="M54" s="12">
-        <f>H54*$V$2+I54*$W$2+J54*$X$2+K54*$Y$2+L54*$Z$2</f>
+        <f t="shared" si="7"/>
         <v>0.9375</v>
       </c>
       <c r="N54" s="13">
@@ -3542,7 +3526,7 @@
         <v>0</v>
       </c>
       <c r="M55" s="12">
-        <f>H55*$V$2+I55*$W$2+J55*$X$2+K55*$Y$2+L55*$Z$2</f>
+        <f t="shared" si="7"/>
         <v>3.75</v>
       </c>
       <c r="N55" s="13">
@@ -3593,7 +3577,7 @@
         <v>0</v>
       </c>
       <c r="M56" s="12">
-        <f>H56*$V$2+I56*$W$2+J56*$X$2+K56*$Y$2+L56*$Z$2</f>
+        <f t="shared" si="7"/>
         <v>26.25</v>
       </c>
       <c r="N56" s="13">
@@ -3644,7 +3628,7 @@
         <v>0</v>
       </c>
       <c r="M57" s="34">
-        <f>H57*$V$2+I57*$W$2+J57*$X$2+K57*$Y$2+L57*$Z$2</f>
+        <f t="shared" si="7"/>
         <v>4.6875</v>
       </c>
       <c r="N57" s="35"/>
@@ -3693,7 +3677,7 @@
         <v>0</v>
       </c>
       <c r="M58" s="34">
-        <f>H58*$V$2+I58*$W$2+J58*$X$2+K58*$Y$2+L58*$Z$2</f>
+        <f t="shared" si="7"/>
         <v>2.8125</v>
       </c>
       <c r="N58" s="35"/>
@@ -3793,7 +3777,7 @@
         <v>0</v>
       </c>
       <c r="M60" s="12">
-        <f>H60*$V$2+I60*$W$2+J60*$X$2+K60*$Y$2+L60*$Z$2</f>
+        <f t="shared" ref="M60:M66" si="8">H60*$V$2+I60*$W$2+J60*$X$2+K60*$Y$2+L60*$Z$2</f>
         <v>26.25</v>
       </c>
       <c r="N60" s="13">
@@ -3844,7 +3828,7 @@
         <v>0</v>
       </c>
       <c r="M61" s="12">
-        <f>H61*$V$2+I61*$W$2+J61*$X$2+K61*$Y$2+L61*$Z$2</f>
+        <f t="shared" si="8"/>
         <v>25.3125</v>
       </c>
       <c r="N61" s="13">
@@ -3895,7 +3879,7 @@
         <v>0</v>
       </c>
       <c r="M62" s="12">
-        <f>H62*$V$2+I62*$W$2+J62*$X$2+K62*$Y$2+L62*$Z$2</f>
+        <f t="shared" si="8"/>
         <v>27.1875</v>
       </c>
       <c r="N62" s="13">
@@ -3946,7 +3930,7 @@
         <v>0</v>
       </c>
       <c r="M63" s="12">
-        <f>H63*$V$2+I63*$W$2+J63*$X$2+K63*$Y$2+L63*$Z$2</f>
+        <f t="shared" si="8"/>
         <v>9.8000000000000007</v>
       </c>
       <c r="N63" s="13">
@@ -3997,7 +3981,7 @@
         <v>0</v>
       </c>
       <c r="M64" s="12">
-        <f>H64*$V$2+I64*$W$2+J64*$X$2+K64*$Y$2+L64*$Z$2</f>
+        <f t="shared" si="8"/>
         <v>45</v>
       </c>
       <c r="N64" s="13">
@@ -4048,7 +4032,7 @@
         <v>0</v>
       </c>
       <c r="M65" s="12">
-        <f>H65*$V$2+I65*$W$2+J65*$X$2+K65*$Y$2+L65*$Z$2</f>
+        <f t="shared" si="8"/>
         <v>26.25</v>
       </c>
       <c r="N65" s="13">
@@ -4099,7 +4083,7 @@
         <v>0</v>
       </c>
       <c r="M66" s="12">
-        <f>H66*$V$2+I66*$W$2+J66*$X$2+K66*$Y$2+L66*$Z$2</f>
+        <f t="shared" si="8"/>
         <v>28.125</v>
       </c>
       <c r="N66" s="13">
@@ -4127,11 +4111,11 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F67" s="19">
-        <f t="shared" ref="F67:F68" si="3">E67*24 -D67*24</f>
+        <f t="shared" ref="F67:F68" si="9">E67*24 -D67*24</f>
         <v>10</v>
       </c>
       <c r="G67" s="20">
-        <f t="shared" ref="G67:G68" si="4">IF(F67 &lt; 0,24+F67,F67)</f>
+        <f t="shared" ref="G67:G68" si="10">IF(F67 &lt; 0,24+F67,F67)</f>
         <v>10</v>
       </c>
       <c r="H67" s="12">
@@ -4150,14 +4134,14 @@
         <v>0</v>
       </c>
       <c r="M67" s="12">
-        <f t="shared" ref="M67:M68" si="5">H67*$V$2+I67*$W$2+J67*$X$2+K67*$Y$2+L67*$Z$2</f>
+        <f t="shared" ref="M67:M68" si="11">H67*$V$2+I67*$W$2+J67*$X$2+K67*$Y$2+L67*$Z$2</f>
         <v>39.375</v>
       </c>
       <c r="N67" s="13">
         <v>39.375</v>
       </c>
       <c r="O67" s="21" t="str">
-        <f t="shared" ref="O67:O68" si="6">IF(M67=N67, "ok", "mismatch")</f>
+        <f t="shared" ref="O67:O68" si="12">IF(M67=N67, "ok", "mismatch")</f>
         <v>ok</v>
       </c>
     </row>
@@ -4178,11 +4162,11 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F68" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="G68" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="H68" s="12">
@@ -4201,14 +4185,14 @@
         <v>0</v>
       </c>
       <c r="M68" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>30</v>
       </c>
       <c r="N68" s="13">
         <v>30</v>
       </c>
       <c r="O68" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>ok</v>
       </c>
     </row>

</xml_diff>